<commit_message>
Upload Product Focus + Fixing
</commit_message>
<xml_diff>
--- a/public/imports/timegone/032018.xlsx
+++ b/public/imports/timegone/032018.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="34">
   <si>
     <t>ID</t>
   </si>
@@ -34,6 +34,96 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
   </si>
 </sst>
 </file>
@@ -420,7 +510,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2:C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,247 +539,337 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3">
-        <v>2</v>
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <v>3</v>
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>4</v>
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <v>5</v>
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7">
-        <v>6</v>
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8">
-        <v>7</v>
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <v>8</v>
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10">
-        <v>9</v>
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11">
-        <v>10</v>
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12">
-        <v>11</v>
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13">
-        <v>12</v>
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B14">
-        <v>13</v>
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15">
-        <v>14</v>
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16">
-        <v>15</v>
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
       </c>
       <c r="C16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17">
-        <v>16</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
       </c>
       <c r="C17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18">
-        <v>17</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
       </c>
       <c r="C18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19">
-        <v>18</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
       </c>
       <c r="C19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20">
-        <v>19</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
       </c>
       <c r="C20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21">
-        <v>20</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
       </c>
       <c r="C21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22">
-        <v>21</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
+        <v>23</v>
       </c>
       <c r="C22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23">
-        <v>22</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>24</v>
       </c>
       <c r="C23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24">
-        <v>23</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
       </c>
       <c r="C24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25">
-        <v>24</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
       </c>
       <c r="C25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26">
-        <v>25</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" t="s">
+        <v>27</v>
       </c>
       <c r="C26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27">
-        <v>26</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" t="s">
+        <v>28</v>
       </c>
       <c r="C27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28">
-        <v>27</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" t="s">
+        <v>29</v>
       </c>
       <c r="C28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29">
-        <v>28</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" t="s">
+        <v>30</v>
       </c>
       <c r="C29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30">
-        <v>29</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" t="s">
+        <v>31</v>
       </c>
       <c r="C30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31">
-        <v>30</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" t="s">
+        <v>32</v>
       </c>
       <c r="C31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32">
-        <v>31</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" t="s">
+        <v>33</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>